<commit_message>
add `0` to vaccination dose for 12-17 and 11-
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05031018.xlsx
+++ b/data/vaccine/vaccination_12dose_05031018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48477C58-0213-664B-8DB9-544236A61DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFC1273-D495-574D-839D-54DC1AF4966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23580" yWindow="2120" windowWidth="21300" windowHeight="13680" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="19660" yWindow="2120" windowWidth="21300" windowHeight="13680" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,8 +551,12 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
@@ -579,8 +583,12 @@
       <c r="A2" s="1">
         <v>44319</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
       <c r="D2" s="2">
         <v>159618</v>
       </c>
@@ -607,8 +615,12 @@
       <c r="A3" s="1">
         <v>44326</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
       <c r="D3" s="2">
         <v>160322</v>
       </c>
@@ -635,8 +647,12 @@
       <c r="A4" s="1">
         <v>44333</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
       <c r="D4" s="2">
         <v>161073</v>
       </c>
@@ -663,8 +679,12 @@
       <c r="A5" s="1">
         <v>44340</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
       <c r="D5" s="2">
         <v>161823</v>
       </c>
@@ -691,8 +711,12 @@
       <c r="A6" s="1">
         <v>44347</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
       <c r="D6" s="2">
         <v>163333</v>
       </c>
@@ -719,8 +743,12 @@
       <c r="A7" s="1">
         <v>44354</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
       <c r="D7" s="2">
         <v>165863</v>
       </c>
@@ -747,8 +775,12 @@
       <c r="A8" s="1">
         <v>44361</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
       <c r="D8" s="2">
         <v>314874</v>
       </c>
@@ -775,8 +807,12 @@
       <c r="A9" s="1">
         <v>44368</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
       <c r="D9" s="2">
         <v>553889</v>
       </c>
@@ -803,8 +839,12 @@
       <c r="A10" s="1">
         <v>44375</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
       <c r="D10" s="2">
         <v>774868</v>
       </c>
@@ -831,8 +871,12 @@
       <c r="A11" s="1">
         <v>44382</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
       <c r="D11" s="2">
         <v>796911</v>
       </c>
@@ -859,8 +903,12 @@
       <c r="A12" s="1">
         <v>44389</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
       <c r="D12" s="2">
         <v>886035</v>
       </c>
@@ -887,8 +935,12 @@
       <c r="A13" s="1">
         <v>44396</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
       <c r="D13" s="2">
         <v>951053</v>
       </c>
@@ -915,8 +967,12 @@
       <c r="A14" s="1">
         <v>44403</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
       <c r="D14" s="2">
         <v>1400634</v>
       </c>
@@ -943,8 +999,12 @@
       <c r="A15" s="1">
         <v>44410</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
       <c r="D15" s="2">
         <v>1759173</v>
       </c>
@@ -971,8 +1031,12 @@
       <c r="A16" s="1">
         <v>44417</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
       <c r="D16" s="2">
         <v>1978965</v>
       </c>
@@ -999,8 +1063,12 @@
       <c r="A17" s="1">
         <v>44424</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
       <c r="D17" s="2">
         <v>2234899</v>
       </c>
@@ -1027,7 +1095,9 @@
       <c r="A18" s="1">
         <v>44431</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
       <c r="C18" s="2">
         <v>15273</v>
       </c>
@@ -1057,7 +1127,9 @@
       <c r="A19" s="1">
         <v>44438</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
       <c r="C19" s="2">
         <v>15287</v>
       </c>
@@ -1087,7 +1159,9 @@
       <c r="A20" s="1">
         <v>44445</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
       <c r="C20" s="2">
         <v>15290</v>
       </c>
@@ -1117,7 +1191,9 @@
       <c r="A21" s="1">
         <v>44452</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
       <c r="C21" s="2">
         <v>15300</v>
       </c>
@@ -1147,6 +1223,9 @@
       <c r="A22" s="1">
         <v>44459</v>
       </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
       <c r="C22" s="2">
         <v>16311</v>
       </c>
@@ -1176,6 +1255,9 @@
       <c r="A23" s="1">
         <v>44466</v>
       </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
       <c r="C23" s="2">
         <v>16338</v>
       </c>
@@ -1205,6 +1287,9 @@
       <c r="A24" s="1">
         <v>44473</v>
       </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
       <c r="C24" s="2">
         <v>16395</v>
       </c>
@@ -1234,6 +1319,9 @@
       <c r="A25" s="1">
         <v>44480</v>
       </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
       <c r="C25" s="2">
         <v>16613</v>
       </c>
@@ -1262,6 +1350,9 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44487</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
       </c>
       <c r="C26" s="2">
         <v>16949</v>
@@ -1299,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1470,8 +1561,12 @@
       <c r="A11" s="1">
         <v>44382</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
       <c r="D11" s="2">
         <f>310844-17</f>
         <v>310827</v>
@@ -1505,8 +1600,12 @@
       <c r="A12" s="1">
         <v>44389</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
       <c r="D12" s="2">
         <f>537578-18</f>
         <v>537560</v>
@@ -1540,8 +1639,12 @@
       <c r="A13" s="1">
         <v>44396</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
       <c r="D13" s="2">
         <f>742006-18</f>
         <v>741988</v>
@@ -1575,8 +1678,12 @@
       <c r="A14" s="1">
         <v>44403</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
       <c r="D14" s="3">
         <f>754939</f>
         <v>754939</v>
@@ -1610,8 +1717,12 @@
       <c r="A15" s="1">
         <v>44410</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
       <c r="D15" s="2">
         <f>854927-18</f>
         <v>854909</v>
@@ -1645,8 +1756,12 @@
       <c r="A16" s="1">
         <v>44417</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
       <c r="D16" s="3">
         <f>883966</f>
         <v>883966</v>
@@ -1680,8 +1795,12 @@
       <c r="A17" s="1">
         <v>44424</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
       <c r="D17" s="2">
         <f>1379694-18</f>
         <v>1379676</v>
@@ -1715,7 +1834,9 @@
       <c r="A18" s="1">
         <v>44431</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
       <c r="C18" s="2">
         <v>12596</v>
       </c>
@@ -1752,7 +1873,9 @@
       <c r="A19" s="1">
         <v>44438</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
       <c r="C19" s="2">
         <v>13051</v>
       </c>
@@ -1789,7 +1912,9 @@
       <c r="A20" s="1">
         <v>44445</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
       <c r="C20" s="2">
         <v>13243</v>
       </c>
@@ -1826,7 +1951,9 @@
       <c r="A21" s="1">
         <v>44452</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
       <c r="C21" s="2">
         <v>14961</v>
       </c>
@@ -1863,6 +1990,9 @@
       <c r="A22" s="1">
         <v>44459</v>
       </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
       <c r="C22" s="2">
         <v>15805</v>
       </c>
@@ -1899,6 +2029,9 @@
       <c r="A23" s="1">
         <v>44466</v>
       </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
       <c r="C23" s="2">
         <v>15853</v>
       </c>
@@ -1935,6 +2068,9 @@
       <c r="A24" s="1">
         <v>44473</v>
       </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
       <c r="C24" s="2">
         <v>15926</v>
       </c>
@@ -1971,6 +2107,9 @@
       <c r="A25" s="1">
         <v>44480</v>
       </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
       <c r="C25" s="2">
         <v>16053</v>
       </c>
@@ -2006,6 +2145,9 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44487</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
       </c>
       <c r="C26" s="2">
         <v>16163</v>

</xml_diff>

<commit_message>
delete number of vaccination of 12-17 for 2nd dose
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05031018.xlsx
+++ b/data/vaccine/vaccination_12dose_05031018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFC1273-D495-574D-839D-54DC1AF4966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D44B2F-17AB-9A4E-AE42-64C3BA07B3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19660" yWindow="2120" windowWidth="21300" windowHeight="13680" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="19660" yWindow="2120" windowWidth="21300" windowHeight="13680" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>12596</v>
+        <v>0</v>
       </c>
       <c r="D18" s="3">
         <f>1445177-19</f>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>13051</v>
+        <v>0</v>
       </c>
       <c r="D19" s="3">
         <f>1465804-22</f>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <v>13243</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2">
         <f>1584973-43</f>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>14961</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
         <f>1912209-66</f>

</xml_diff>